<commit_message>
Correcciones gestion de la produccion 1
</commit_message>
<xml_diff>
--- a/Proyecto 70%/Nueva Planta/Tiempos Falla y KPI Planta Nueva.xlsx
+++ b/Proyecto 70%/Nueva Planta/Tiempos Falla y KPI Planta Nueva.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive - Universidad Nacional de Colombia\Escritorio\Semestre 16\APM\Proyecto\STEELO\Proyecto 70%\Nueva Planta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B906C98-6B95-4378-84FE-CF8DFB77FA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411CD99C-E5A8-4C90-84F7-954B7F260BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Falla" sheetId="1" r:id="rId1"/>
     <sheet name="KPIs" sheetId="2" r:id="rId2"/>
+    <sheet name="Plant" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="91">
   <si>
     <t>Jornada</t>
   </si>
@@ -79,9 +80,6 @@
   </si>
   <si>
     <t>https://hpclaser.co.uk/how-to-maintain-and-service-your-laser-machine-effectively/</t>
-  </si>
-  <si>
-    <t>Dobladora Manual</t>
   </si>
   <si>
     <t>https://www.harsle.com/Bending-machine-maintenance-and-use-id1118886.html#:~:text=After%20the%20new%20machine%20is,fuel%20tank%20should%20be%20cleaned.&amp;text=The%20system%20oil%20temperature%20should,not%20exceed%2070%20%C2%B0C.</t>
@@ -301,16 +299,68 @@
   <si>
     <t>Pintura celda robotizada</t>
   </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Portion</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Mean Value</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>limpieza</t>
+  </si>
+  <si>
+    <t>CorteCNC</t>
+  </si>
+  <si>
+    <t>1:05:01:31.3362</t>
+  </si>
+  <si>
+    <t>Doblado2</t>
+  </si>
+  <si>
+    <t>Pintura</t>
+  </si>
+  <si>
+    <t>Horno</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Failed Time</t>
+  </si>
+  <si>
+    <t>Piezas mensua</t>
+  </si>
+  <si>
+    <t>Hras mes</t>
+  </si>
+  <si>
+    <t>Dobladora CNC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="172" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +396,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,8 +423,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCDCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -759,13 +828,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF464646"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF464646"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF464646"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF464646"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -790,6 +931,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -798,15 +966,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -826,15 +985,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -842,15 +992,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -873,6 +1014,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="47" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1157,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,18 +1336,18 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
+      <c r="A2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
+      <c r="A3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1249,7 +1415,7 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1">
         <f>4*2</f>
@@ -1271,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,63 +1495,63 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1">
         <v>5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1">
         <v>40</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B19" s="8">
         <v>5</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="11">
         <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:5" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1440,7 +1606,7 @@
     </row>
     <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1">
         <f>+(2+2+1+2+2)*12</f>
@@ -1452,7 +1618,7 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
         <v>16</v>
@@ -1473,7 +1639,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,63 +1697,63 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="1">
         <v>40</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="8">
         <v>10</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="11">
         <v>2</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:3" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
+      <c r="A44" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="33"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -1632,7 +1798,7 @@
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1">
         <f>(1)*4*12</f>
@@ -1644,7 +1810,7 @@
     </row>
     <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" s="1">
         <f>+(2+2+2)*12</f>
@@ -1656,7 +1822,7 @@
     </row>
     <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="1">
         <v>8</v>
@@ -1667,7 +1833,7 @@
     </row>
     <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="1">
         <f>12*4</f>
@@ -1732,71 +1898,71 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="1">
-        <f>14*8</f>
-        <v>112</v>
+        <f>B59*8</f>
+        <v>16</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="8">
         <v>10</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="11">
         <v>5</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:3" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="35"/>
+      <c r="C65" s="36"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="30"/>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="33"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="39"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="30"/>
+      <c r="A67" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="35"/>
+      <c r="C67" s="36"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
@@ -1853,7 +2019,7 @@
     </row>
     <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B73" s="1">
         <f>(1)*12</f>
@@ -1865,7 +2031,7 @@
     </row>
     <row r="74" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" s="1">
         <f>3*4</f>
@@ -1942,67 +2108,67 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" s="1">
         <f>20/8</f>
         <v>2.5</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B82" s="1">
         <v>20</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B83" s="8">
         <v>5</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B85" s="11">
         <v>2</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="22"/>
-      <c r="B87" s="23"/>
-      <c r="C87" s="24"/>
+      <c r="A87" s="31"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="33"/>
     </row>
     <row r="88" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="B88" s="35"/>
-      <c r="C88" s="36"/>
+      <c r="A88" s="25"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="27"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B89" s="26"/>
-      <c r="C89" s="27"/>
+      <c r="A89" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" s="23"/>
+      <c r="C89" s="24"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
@@ -2032,7 +2198,7 @@
     </row>
     <row r="94" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="5"/>
@@ -2046,14 +2212,14 @@
     </row>
     <row r="96" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="5"/>
     </row>
     <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="5"/>
@@ -2067,8 +2233,12 @@
       <c r="A99" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="5"/>
+      <c r="B99" s="1">
+        <v>60</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
@@ -2081,7 +2251,9 @@
       <c r="A101" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="1"/>
+      <c r="B101" s="63">
+        <v>0.98</v>
+      </c>
       <c r="C101" s="5"/>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2093,67 +2265,67 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B103" s="1">
         <v>5.5</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B104" s="1">
         <f>B103*8</f>
         <v>44</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B105" s="8">
         <v>7</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B107" s="11"/>
       <c r="C107" s="12"/>
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B109" s="23"/>
-      <c r="C109" s="24"/>
+      <c r="A109" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B109" s="32"/>
+      <c r="C109" s="33"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B110" s="35"/>
-      <c r="C110" s="36"/>
+      <c r="A110" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" s="26"/>
+      <c r="C110" s="27"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B111" s="26"/>
-      <c r="C111" s="27"/>
+      <c r="A111" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" s="23"/>
+      <c r="C111" s="24"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
@@ -2198,7 +2370,7 @@
     </row>
     <row r="116" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B116" s="1">
         <f>(2)*4*12</f>
@@ -2222,7 +2394,7 @@
     </row>
     <row r="118" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B118" s="1">
         <f>3*8</f>
@@ -2299,70 +2471,70 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B125" s="1">
         <v>45</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B126" s="1">
         <v>45</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B127" s="8">
         <v>7</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B129" s="11">
         <v>5</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="131" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B131" s="23"/>
-      <c r="C131" s="24"/>
+      <c r="A131" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B131" s="32"/>
+      <c r="C131" s="33"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B132" s="35"/>
-      <c r="C132" s="36"/>
+      <c r="A132" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B132" s="26"/>
+      <c r="C132" s="27"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B133" s="26"/>
-      <c r="C133" s="27"/>
+      <c r="A133" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B133" s="23"/>
+      <c r="C133" s="24"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
@@ -2431,7 +2603,7 @@
     </row>
     <row r="140" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B140" s="1">
         <f>1*12</f>
@@ -2508,71 +2680,71 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B147" s="1">
         <f>B148/8</f>
         <v>1.25</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B148" s="1">
         <v>10</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B149" s="8">
         <v>5</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="151" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B151" s="11">
         <v>2</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="153" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="22" t="s">
+      <c r="A153" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B153" s="32"/>
+      <c r="C153" s="33"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B153" s="23"/>
-      <c r="C153" s="24"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B154" s="35"/>
-      <c r="C154" s="36"/>
+      <c r="B154" s="26"/>
+      <c r="C154" s="27"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B155" s="26"/>
-      <c r="C155" s="27"/>
+      <c r="A155" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B155" s="23"/>
+      <c r="C155" s="24"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
@@ -2641,7 +2813,7 @@
     </row>
     <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B162" s="1">
         <f>3*8</f>
@@ -2718,71 +2890,71 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B169" s="1">
         <f>B170/8</f>
         <v>1.25</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B170" s="1">
         <v>10</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B171" s="8">
         <v>5</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="173" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B173" s="11">
         <v>2</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="175" spans="1:3" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B175" s="23"/>
-      <c r="C175" s="24"/>
+      <c r="A175" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B175" s="32"/>
+      <c r="C175" s="33"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B176" s="38"/>
-      <c r="C176" s="39"/>
+      <c r="A176" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B176" s="41"/>
+      <c r="C176" s="42"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="27"/>
+      <c r="A177" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B177" s="23"/>
+      <c r="C177" s="24"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
@@ -2851,7 +3023,7 @@
     </row>
     <row r="184" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B184" s="1">
         <f>3*8</f>
@@ -2928,60 +3100,52 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B191" s="1">
         <v>2</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B192" s="1">
         <v>16</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B193" s="8">
         <v>2</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="195" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B195" s="11">
         <v>2</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A87:C87"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A131:C131"/>
@@ -2998,6 +3162,14 @@
     <mergeCell ref="A175:C175"/>
     <mergeCell ref="A176:C176"/>
     <mergeCell ref="A132:C132"/>
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A87:C87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A44" r:id="rId1" location=":~:text=After%20the%20new%20machine%20is,fuel%20tank%20should%20be%20cleaned.&amp;text=The%20system%20oil%20temperature%20should,not%20exceed%2070%20%C2%B0C." xr:uid="{60422AFF-22B2-403F-97A6-7C111BF5F0D1}"/>
@@ -3014,10 +3186,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C3A3D7-0B25-4D19-96A3-8CC1F6FCF3A9}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,76 +3197,76 @@
     <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
       <c r="D1" s="46">
         <f>D3*D11*D20</f>
-        <v>0.35139866666666669</v>
+        <v>0.25032183749999998</v>
       </c>
       <c r="E1" s="44"/>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
       <c r="D3" s="47">
         <f>E9/E7</f>
-        <v>0.88</v>
+        <v>0.54</v>
       </c>
       <c r="E3" s="44"/>
     </row>
-    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>50</v>
-      </c>
       <c r="B5" s="18">
-        <f>5.5*4*12</f>
-        <v>264</v>
+        <f>5*4*12</f>
+        <v>240</v>
       </c>
       <c r="C5" s="18">
         <f t="shared" ref="C5" si="0">B5*24</f>
-        <v>6336</v>
+        <v>5760</v>
       </c>
       <c r="D5" s="18">
         <f t="shared" ref="D5:E5" si="1">C5*60</f>
-        <v>380160</v>
+        <v>345600</v>
       </c>
       <c r="E5" s="18">
         <f t="shared" si="1"/>
-        <v>22809600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20736000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="18">
         <f>B5-B7</f>
@@ -3102,147 +3274,163 @@
       </c>
       <c r="C6" s="18">
         <f>C5-C7</f>
-        <v>3696</v>
+        <v>3360</v>
       </c>
       <c r="D6" s="18">
         <f>D5-D7</f>
-        <v>221760</v>
+        <v>201600</v>
       </c>
       <c r="E6" s="18">
         <f>E5-E7</f>
-        <v>13305600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12096000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="19">
-        <f>5.5*4*12</f>
-        <v>264</v>
+        <f>5*4*12</f>
+        <v>240</v>
       </c>
       <c r="C7" s="18">
         <f>B7*10</f>
-        <v>2640</v>
+        <v>2400</v>
       </c>
       <c r="D7" s="19">
         <f>C7*60</f>
-        <v>158400</v>
+        <v>144000</v>
       </c>
       <c r="E7" s="19">
         <f>D7*60</f>
-        <v>9504000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8640000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="18">
-        <f>B7*0.12</f>
-        <v>31.68</v>
+        <f>C8/10</f>
+        <v>110.4</v>
       </c>
       <c r="C8" s="18">
-        <f>B8*10</f>
-        <v>316.8</v>
+        <f>Plant!D11+C7*0.05</f>
+        <v>1104</v>
       </c>
       <c r="D8" s="18">
         <f>C8*60</f>
-        <v>19008</v>
+        <v>66240</v>
       </c>
       <c r="E8" s="18">
         <f>D8*60</f>
-        <v>1140480</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3974400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="19">
         <f t="shared" ref="B9:D9" si="2">B7-B8</f>
-        <v>232.32</v>
+        <v>129.6</v>
       </c>
       <c r="C9" s="19">
         <f t="shared" si="2"/>
-        <v>2323.1999999999998</v>
+        <v>1296</v>
       </c>
       <c r="D9" s="19">
         <f t="shared" si="2"/>
-        <v>139392</v>
+        <v>77760</v>
       </c>
       <c r="E9" s="19">
         <f>E7-E8</f>
-        <v>8363520</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4665600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
       <c r="E10" s="44"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
       <c r="D11" s="49">
         <f>E15*E18</f>
-        <v>0.41166666666666668</v>
+        <v>0.4778958333333333</v>
       </c>
       <c r="E11" s="50"/>
     </row>
-    <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="20">
-        <f>38*B5*D3</f>
-        <v>8828.16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>G13*12</f>
+        <v>9492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="20">
-        <f>(10*60*60)/38</f>
-        <v>947.36842105263156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="58">
+        <f>G14/G13*60*60</f>
+        <v>910.24020227560038</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="60">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="18">
         <f t="shared" ref="B14:E14" si="3">B9</f>
-        <v>232.32</v>
+        <v>129.6</v>
       </c>
       <c r="C14" s="18">
         <f t="shared" si="3"/>
-        <v>2323.1999999999998</v>
+        <v>1296</v>
       </c>
       <c r="D14" s="18">
         <f t="shared" si="3"/>
-        <v>139392</v>
-      </c>
-      <c r="E14" s="20">
-        <f t="shared" si="3"/>
-        <v>8363520</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77760</v>
+      </c>
+      <c r="E14" s="58">
+        <f>E7</f>
+        <v>8640000</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="62">
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <f>52/8+0.75</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="19">
         <f t="shared" ref="B15:E15" si="4">B12*B13/B14</f>
@@ -3258,19 +3446,23 @@
       </c>
       <c r="E15" s="21">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="J15">
+        <f>J14*60</f>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="20">
-        <f>MIN((2+2+Falla!B18+Falla!B19+Falla!B21*8+Falla!B39+Falla!B40+Falla!B42*8+Falla!B60+Falla!B61+Falla!B63*8+Falla!B82+Falla!B83+Falla!B85*8+Falla!B104+Falla!B105+Falla!B107*8+Falla!B126+Falla!B127+Falla!B129*8+Falla!B148+Falla!B149+Falla!B151*8+Falla!B170+Falla!B171+Falla!B173*8+Falla!B192+Falla!B193+Falla!B195*8)/8,MAX(Falla!B17,Falla!B38,Falla!B59,Falla!B81,Falla!B103,Falla!B147,Falla!B169,Falla!B191))*0+52/8*60</f>
-        <v>390</v>
+        <f>J15</f>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3292,19 +3484,19 @@
       </c>
       <c r="E17" s="20">
         <f t="shared" si="5"/>
-        <v>947.36842105263156</v>
+        <v>910.24020227560038</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="21">
         <f>E16/E17</f>
-        <v>0.41166666666666668</v>
+        <v>0.47789583333333341</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3316,7 +3508,7 @@
     </row>
     <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -3341,4 +3533,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD9B8BC-AFA4-4DC9-B831-69D0BB7D953B}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="53">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="C2" s="54">
+        <v>6</v>
+      </c>
+      <c r="D2" s="57">
+        <v>0.46616535879629634</v>
+      </c>
+      <c r="E2" s="55">
+        <v>7.7694224537037046E-2</v>
+      </c>
+      <c r="F2" s="55">
+        <v>7.3408449074074067E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="53">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="C3" s="54">
+        <v>12</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="55">
+        <v>0.10078253472222222</v>
+      </c>
+      <c r="F3" s="55">
+        <v>4.5562581018518518E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="53">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="C4" s="54">
+        <v>8</v>
+      </c>
+      <c r="D4" s="57">
+        <v>0.19651340277777776</v>
+      </c>
+      <c r="E4" s="55">
+        <v>2.4564178240740739E-2</v>
+      </c>
+      <c r="F4" s="55">
+        <v>2.0624189814814814E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="53">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="C5" s="54">
+        <v>6</v>
+      </c>
+      <c r="D5" s="57">
+        <v>0.36017188657407412</v>
+      </c>
+      <c r="E5" s="55">
+        <v>6.0028645833333338E-2</v>
+      </c>
+      <c r="F5" s="55">
+        <v>3.285208333333333E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="53">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="C6" s="54">
+        <v>1</v>
+      </c>
+      <c r="D6" s="57">
+        <v>9.2675810185185187E-3</v>
+      </c>
+      <c r="E6" s="55">
+        <v>9.2675810185185187E-3</v>
+      </c>
+      <c r="F6" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="53">
+        <v>6.7299999999999999E-2</v>
+      </c>
+      <c r="C7" s="54">
+        <v>4</v>
+      </c>
+      <c r="D7" s="57">
+        <v>0.56088188657407401</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0.14022047453703704</v>
+      </c>
+      <c r="F7" s="55">
+        <v>9.7589513888888882E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="53">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="C8" s="54">
+        <v>11</v>
+      </c>
+      <c r="D8" s="57">
+        <v>0.17850421296296295</v>
+      </c>
+      <c r="E8" s="55">
+        <v>1.6227650462962963E-2</v>
+      </c>
+      <c r="F8" s="55">
+        <v>1.4805393518518518E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="53">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="C9" s="54">
+        <v>12</v>
+      </c>
+      <c r="D9" s="57">
+        <v>0.63553975694444442</v>
+      </c>
+      <c r="E9" s="55">
+        <v>5.2961643518518516E-2</v>
+      </c>
+      <c r="F9" s="55">
+        <v>2.8782152777777778E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="53">
+        <v>3.8899999999999997E-2</v>
+      </c>
+      <c r="C10" s="54">
+        <v>17</v>
+      </c>
+      <c r="D10" s="57">
+        <v>0.32432623842592595</v>
+      </c>
+      <c r="E10" s="55">
+        <v>1.907800925925926E-2</v>
+      </c>
+      <c r="F10" s="55">
+        <v>1.3607766203703705E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <f>(11+29+5+8.5+12+1.5+4+3+8)*12</f>
+        <v>984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion y correcciones gestion de la produccion 2
</commit_message>
<xml_diff>
--- a/Proyecto 70%/Nueva Planta/Tiempos Falla y KPI Planta Nueva.xlsx
+++ b/Proyecto 70%/Nueva Planta/Tiempos Falla y KPI Planta Nueva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive - Universidad Nacional de Colombia\Escritorio\Semestre 16\APM\Proyecto\STEELO\Proyecto 70%\Nueva Planta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411CD99C-E5A8-4C90-84F7-954B7F260BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D8EDB4-B89F-4E85-81E4-33FC72EA6D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="14760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Falla" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="90">
   <si>
     <t>Jornada</t>
   </si>
@@ -324,9 +324,6 @@
     <t>CorteCNC</t>
   </si>
   <si>
-    <t>1:05:01:31.3362</t>
-  </si>
-  <si>
     <t>Doblado2</t>
   </si>
   <si>
@@ -358,7 +355,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="172" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -931,6 +928,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="47" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -939,33 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -985,6 +989,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -992,6 +1005,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,31 +1036,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="47" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1336,18 +1333,18 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1540,18 +1537,18 @@
     </row>
     <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:5" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="40"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1742,18 +1739,18 @@
     </row>
     <row r="43" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:3" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="33"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
+      <c r="A45" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="39"/>
+      <c r="C45" s="40"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -1944,25 +1941,25 @@
     </row>
     <row r="64" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:3" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="35"/>
-      <c r="C65" s="36"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="43"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="39"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="46"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="36"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="43"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
@@ -2154,21 +2151,21 @@
     </row>
     <row r="86" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="31"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="33"/>
+      <c r="A87" s="35"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="37"/>
     </row>
     <row r="88" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="27"/>
+      <c r="A88" s="47"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="49"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B89" s="23"/>
-      <c r="C89" s="24"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="40"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
@@ -2251,7 +2248,7 @@
       <c r="A101" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="63">
+      <c r="B101" s="34">
         <v>0.98</v>
       </c>
       <c r="C101" s="5"/>
@@ -2307,25 +2304,25 @@
     </row>
     <row r="108" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="109" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="31" t="s">
+      <c r="A109" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B109" s="32"/>
-      <c r="C109" s="33"/>
+      <c r="B109" s="36"/>
+      <c r="C109" s="37"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B110" s="26"/>
-      <c r="C110" s="27"/>
+      <c r="B110" s="48"/>
+      <c r="C110" s="49"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="22" t="s">
+      <c r="A111" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B111" s="23"/>
-      <c r="C111" s="24"/>
+      <c r="B111" s="39"/>
+      <c r="C111" s="40"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
@@ -2516,25 +2513,25 @@
     </row>
     <row r="130" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="131" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="31" t="s">
+      <c r="A131" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B131" s="32"/>
-      <c r="C131" s="33"/>
+      <c r="B131" s="36"/>
+      <c r="C131" s="37"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="25" t="s">
+      <c r="A132" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B132" s="26"/>
-      <c r="C132" s="27"/>
+      <c r="B132" s="48"/>
+      <c r="C132" s="49"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="22" t="s">
+      <c r="A133" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B133" s="23"/>
-      <c r="C133" s="24"/>
+      <c r="B133" s="39"/>
+      <c r="C133" s="40"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
@@ -2726,25 +2723,25 @@
     </row>
     <row r="152" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="153" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="31" t="s">
+      <c r="A153" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B153" s="32"/>
-      <c r="C153" s="33"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="37"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="25" t="s">
+      <c r="A154" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B154" s="26"/>
-      <c r="C154" s="27"/>
+      <c r="B154" s="48"/>
+      <c r="C154" s="49"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="22" t="s">
+      <c r="A155" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B155" s="23"/>
-      <c r="C155" s="24"/>
+      <c r="B155" s="39"/>
+      <c r="C155" s="40"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
@@ -2936,25 +2933,25 @@
     </row>
     <row r="174" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="175" spans="1:3" ht="27" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="31" t="s">
+      <c r="A175" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B175" s="32"/>
-      <c r="C175" s="33"/>
+      <c r="B175" s="36"/>
+      <c r="C175" s="37"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="40" t="s">
+      <c r="A176" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B176" s="41"/>
-      <c r="C176" s="42"/>
+      <c r="B176" s="51"/>
+      <c r="C176" s="52"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="22" t="s">
+      <c r="A177" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B177" s="23"/>
-      <c r="C177" s="24"/>
+      <c r="B177" s="39"/>
+      <c r="C177" s="40"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
@@ -3146,6 +3143,14 @@
     <row r="196" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A87:C87"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A131:C131"/>
@@ -3162,14 +3167,6 @@
     <mergeCell ref="A175:C175"/>
     <mergeCell ref="A176:C176"/>
     <mergeCell ref="A132:C132"/>
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A87:C87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A44" r:id="rId1" location=":~:text=After%20the%20new%20machine%20is,fuel%20tank%20should%20be%20cleaned.&amp;text=The%20system%20oil%20temperature%20should,not%20exceed%2070%20%C2%B0C." xr:uid="{60422AFF-22B2-403F-97A6-7C111BF5F0D1}"/>
@@ -3188,8 +3185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C3A3D7-0B25-4D19-96A3-8CC1F6FCF3A9}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,16 +3195,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="46">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="59">
         <f>D3*D11*D20</f>
-        <v>0.25032183749999998</v>
-      </c>
-      <c r="E1" s="44"/>
+        <v>0.51816187499999999</v>
+      </c>
+      <c r="E1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -3217,16 +3214,16 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="47">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="60">
         <f>E9/E7</f>
-        <v>0.54</v>
-      </c>
-      <c r="E3" s="44"/>
+        <v>0.66</v>
+      </c>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
@@ -3312,19 +3309,19 @@
       </c>
       <c r="B8" s="18">
         <f>C8/10</f>
-        <v>110.4</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="C8" s="18">
         <f>Plant!D11+C7*0.05</f>
-        <v>1104</v>
+        <v>816</v>
       </c>
       <c r="D8" s="18">
         <f>C8*60</f>
-        <v>66240</v>
+        <v>48960</v>
       </c>
       <c r="E8" s="18">
         <f>D8*60</f>
-        <v>3974400</v>
+        <v>2937600</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3333,39 +3330,39 @@
       </c>
       <c r="B9" s="19">
         <f t="shared" ref="B9:D9" si="2">B7-B8</f>
-        <v>129.6</v>
+        <v>158.4</v>
       </c>
       <c r="C9" s="19">
         <f t="shared" si="2"/>
-        <v>1296</v>
+        <v>1584</v>
       </c>
       <c r="D9" s="19">
         <f t="shared" si="2"/>
-        <v>77760</v>
+        <v>95040</v>
       </c>
       <c r="E9" s="19">
         <f>E7-E8</f>
-        <v>4665600</v>
+        <v>5702400</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="49">
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="62">
         <f>E15*E18</f>
-        <v>0.4778958333333333</v>
-      </c>
-      <c r="E11" s="50"/>
+        <v>0.80937499999999996</v>
+      </c>
+      <c r="E11" s="63"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
@@ -3376,7 +3373,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="20">
         <f>G13*12</f>
-        <v>9492</v>
+        <v>15540</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3386,15 +3383,15 @@
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="58">
+      <c r="E13" s="29">
         <f>G14/G13*60*60</f>
-        <v>910.24020227560038</v>
-      </c>
-      <c r="F13" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="60">
-        <v>791</v>
+        <v>555.98455598455598</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="31">
+        <v>1295</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3402,25 +3399,25 @@
         <v>57</v>
       </c>
       <c r="B14" s="18">
-        <f t="shared" ref="B14:E14" si="3">B9</f>
-        <v>129.6</v>
+        <f t="shared" ref="B14:D14" si="3">B9</f>
+        <v>158.4</v>
       </c>
       <c r="C14" s="18">
         <f t="shared" si="3"/>
-        <v>1296</v>
+        <v>1584</v>
       </c>
       <c r="D14" s="18">
         <f t="shared" si="3"/>
-        <v>77760</v>
-      </c>
-      <c r="E14" s="58">
+        <v>95040</v>
+      </c>
+      <c r="E14" s="29">
         <f>E7</f>
         <v>8640000</v>
       </c>
-      <c r="F14" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="62">
+      <c r="F14" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="33">
         <v>200</v>
       </c>
       <c r="J14">
@@ -3446,7 +3443,7 @@
       </c>
       <c r="E15" s="21">
         <f t="shared" si="4"/>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <f>J14*60</f>
@@ -3461,8 +3458,8 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="20">
-        <f>J15</f>
-        <v>435</v>
+        <f>(52+4+4)/8*60</f>
+        <v>450</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3484,7 +3481,7 @@
       </c>
       <c r="E17" s="20">
         <f t="shared" si="5"/>
-        <v>910.24020227560038</v>
+        <v>555.98455598455598</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3496,7 +3493,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="21">
         <f>E16/E17</f>
-        <v>0.47789583333333341</v>
+        <v>0.80937499999999996</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3507,15 +3504,15 @@
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45">
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58">
         <v>0.97</v>
       </c>
-      <c r="E20" s="44"/>
+      <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3540,7 +3537,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,212 +3546,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="24">
         <v>5.5899999999999998E-2</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="25">
         <v>6</v>
       </c>
-      <c r="D2" s="57">
+      <c r="D2" s="28">
         <v>0.46616535879629634</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="26">
         <v>7.7694224537037046E-2</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="26">
         <v>7.3408449074074067E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="24">
         <v>0.14510000000000001</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="25">
         <v>12</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="28">
+        <v>0.20939046296296296</v>
+      </c>
+      <c r="E3" s="26">
+        <v>0.10078253472222222</v>
+      </c>
+      <c r="F3" s="26">
+        <v>4.5562581018518518E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="55">
-        <v>0.10078253472222222</v>
-      </c>
-      <c r="F3" s="55">
-        <v>4.5562581018518518E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="B4" s="24">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="C4" s="25">
+        <v>8</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0.19651340277777776</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2.4564178240740739E-2</v>
+      </c>
+      <c r="F4" s="26">
+        <v>2.0624189814814814E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="24">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="C5" s="25">
+        <v>6</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0.36017188657407412</v>
+      </c>
+      <c r="E5" s="26">
+        <v>6.0028645833333338E-2</v>
+      </c>
+      <c r="F5" s="26">
+        <v>3.285208333333333E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="53">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="C4" s="54">
-        <v>8</v>
-      </c>
-      <c r="D4" s="57">
-        <v>0.19651340277777776</v>
-      </c>
-      <c r="E4" s="55">
-        <v>2.4564178240740739E-2</v>
-      </c>
-      <c r="F4" s="55">
-        <v>2.0624189814814814E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="53">
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="C5" s="54">
-        <v>6</v>
-      </c>
-      <c r="D5" s="57">
-        <v>0.36017188657407412</v>
-      </c>
-      <c r="E5" s="55">
-        <v>6.0028645833333338E-2</v>
-      </c>
-      <c r="F5" s="55">
-        <v>3.285208333333333E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+      <c r="B6" s="24">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="C6" s="25">
+        <v>1</v>
+      </c>
+      <c r="D6" s="28">
+        <v>9.2675810185185187E-3</v>
+      </c>
+      <c r="E6" s="26">
+        <v>9.2675810185185187E-3</v>
+      </c>
+      <c r="F6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="53">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="C6" s="54">
-        <v>1</v>
-      </c>
-      <c r="D6" s="57">
-        <v>9.2675810185185187E-3</v>
-      </c>
-      <c r="E6" s="55">
-        <v>9.2675810185185187E-3</v>
-      </c>
-      <c r="F6" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="B7" s="24">
+        <v>6.7299999999999999E-2</v>
+      </c>
+      <c r="C7" s="25">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28">
+        <v>0.56088188657407401</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0.14022047453703704</v>
+      </c>
+      <c r="F7" s="26">
+        <v>9.7589513888888882E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="24">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="C8" s="25">
+        <v>11</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0.17850421296296295</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1.6227650462962963E-2</v>
+      </c>
+      <c r="F8" s="26">
+        <v>1.4805393518518518E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="24">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="C9" s="25">
+        <v>12</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0.63553975694444442</v>
+      </c>
+      <c r="E9" s="26">
+        <v>5.2961643518518516E-2</v>
+      </c>
+      <c r="F9" s="26">
+        <v>2.8782152777777778E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="53">
-        <v>6.7299999999999999E-2</v>
-      </c>
-      <c r="C7" s="54">
-        <v>4</v>
-      </c>
-      <c r="D7" s="57">
-        <v>0.56088188657407401</v>
-      </c>
-      <c r="E7" s="55">
-        <v>0.14022047453703704</v>
-      </c>
-      <c r="F7" s="55">
-        <v>9.7589513888888882E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="53">
-        <v>2.1399999999999999E-2</v>
-      </c>
-      <c r="C8" s="54">
-        <v>11</v>
-      </c>
-      <c r="D8" s="57">
-        <v>0.17850421296296295</v>
-      </c>
-      <c r="E8" s="55">
-        <v>1.6227650462962963E-2</v>
-      </c>
-      <c r="F8" s="55">
-        <v>1.4805393518518518E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="53">
-        <v>7.6300000000000007E-2</v>
-      </c>
-      <c r="C9" s="54">
-        <v>12</v>
-      </c>
-      <c r="D9" s="57">
-        <v>0.63553975694444442</v>
-      </c>
-      <c r="E9" s="55">
-        <v>5.2961643518518516E-2</v>
-      </c>
-      <c r="F9" s="55">
-        <v>2.8782152777777778E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52" t="s">
+      <c r="B10" s="24">
+        <v>3.8899999999999997E-2</v>
+      </c>
+      <c r="C10" s="25">
+        <v>17</v>
+      </c>
+      <c r="D10" s="28">
+        <v>0.32432623842592595</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1.907800925925926E-2</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1.3607766203703705E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="53">
-        <v>3.8899999999999997E-2</v>
-      </c>
-      <c r="C10" s="54">
-        <v>17</v>
-      </c>
-      <c r="D10" s="57">
-        <v>0.32432623842592595</v>
-      </c>
-      <c r="E10" s="55">
-        <v>1.907800925925926E-2</v>
-      </c>
-      <c r="F10" s="55">
-        <v>1.3607766203703705E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
-        <v>87</v>
-      </c>
       <c r="D11">
-        <f>(11+29+5+8.5+12+1.5+4+3+8)*12</f>
-        <v>984</v>
+        <f>(11+5+5+8.5+12+1.5+4+3+8)*12</f>
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>